<commit_message>
Updated ICSD3-Queries, ICDS3-HCHS-Mapping, and ICSD3-MROS-Mapping
Added Chronic Insomnia Disorder to queries, mapped Chronic Insomnia
Disorder criteria for HCHS, updated Obstructive Sleep Apnea query and
added/edited mapping for HCHS and MROS
</commit_message>
<xml_diff>
--- a/icsd3-mappings/icsd3-hchs-mapping.xlsx
+++ b/icsd3-mappings/icsd3-hchs-mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>id</t>
   </si>
@@ -30,12 +30,6 @@
     <t>icdadultosa_history</t>
   </si>
   <si>
-    <t>icsdadultosa_psg5events</t>
-  </si>
-  <si>
-    <t>icsdadultosa_psg15events</t>
-  </si>
-  <si>
     <t>definition</t>
   </si>
   <si>
@@ -175,6 +169,54 @@
   </si>
   <si>
     <t>ahi_ge15</t>
+  </si>
+  <si>
+    <t>icsdinsom_history</t>
+  </si>
+  <si>
+    <t>icsdinsom_symptoms</t>
+  </si>
+  <si>
+    <t>slea4</t>
+  </si>
+  <si>
+    <t>Trouble falling asleep</t>
+  </si>
+  <si>
+    <t>slea5</t>
+  </si>
+  <si>
+    <t>Wake up several times at night</t>
+  </si>
+  <si>
+    <t>slea6</t>
+  </si>
+  <si>
+    <t>Wake up earlier than you plan</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>slea10</t>
+  </si>
+  <si>
+    <t>Feel Sleepy during the Day</t>
+  </si>
+  <si>
+    <t>slea9</t>
+  </si>
+  <si>
+    <t>Sleep difficulties make irritable (SLEA9)</t>
+  </si>
+  <si>
+    <t>3,4,5</t>
+  </si>
+  <si>
+    <t>Sleep Apnea defined as Apnea/Hypopnea Index (3% desat) &gt;= 15</t>
+  </si>
+  <si>
+    <t>icsdadultosa_psggt15events</t>
   </si>
 </sst>
 </file>
@@ -512,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -523,7 +565,7 @@
     <col min="1" max="1" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="61.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -532,10 +574,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -546,13 +588,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -560,10 +602,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -574,10 +616,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -588,13 +630,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -602,10 +644,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -616,10 +658,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -630,10 +672,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -644,10 +686,10 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -658,10 +700,10 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -672,10 +714,10 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -686,13 +728,13 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -700,10 +742,10 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" s="2">
         <v>3</v>
@@ -714,10 +756,10 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14" s="2">
         <v>3</v>
@@ -728,10 +770,10 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D15" s="2">
         <v>1</v>
@@ -742,10 +784,10 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" s="2">
         <v>3</v>
@@ -756,13 +798,13 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -770,10 +812,10 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18" s="2">
         <v>3</v>
@@ -784,10 +826,10 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -798,10 +840,10 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
@@ -812,32 +854,112 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22"/>
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C23"/>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>